<commit_message>
Create and Populate Loans Dimensional table
</commit_message>
<xml_diff>
--- a/Dummy Data/Dim_Loans.xlsx
+++ b/Dummy Data/Dim_Loans.xlsx
@@ -5,27 +5,39 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COLLEGE\BITS PILANI\SS 2nd Semester\DW\DW Project\Loan-Data-Warehouse\Dummy Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sem2\Data Warehousing\assigment\Loan-Data-Warehouse\Dummy Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A1CC53-6BBB-4B12-8CE8-98A7E1F1BA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF35F19-CF4A-4964-AE81-003A6FBA27DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$101</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="13">
   <si>
     <t>Loan Key</t>
   </si>
@@ -54,16 +66,16 @@
     <t>Corporate</t>
   </si>
   <si>
-    <t>Educational</t>
-  </si>
-  <si>
     <t>Fixed</t>
   </si>
   <si>
     <t>Floating</t>
   </si>
   <si>
-    <t>Surrogate Key</t>
+    <t>_Source Key</t>
+  </si>
+  <si>
+    <t>Loan Issue date</t>
   </si>
 </sst>
 </file>
@@ -107,9 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,29 +403,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -424,10 +438,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -435,7 +452,7 @@
         <v>101000</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -443,12 +460,18 @@
       <c r="E2">
         <v>96</v>
       </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F65" ca="1" si="0">RAND()*10000 + 100000</f>
-        <v>102195.36616411386</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="2">
+        <v>43536</v>
+      </c>
+      <c r="G2">
+        <v>106485.57</v>
+      </c>
+      <c r="J2" t="str">
+        <f>"INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES ("&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;","&amp;G2&amp;");"</f>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101000,'Floating','Personal',96,106485.57);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -456,7 +479,7 @@
         <v>101001</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -464,12 +487,18 @@
       <c r="E3">
         <v>36</v>
       </c>
-      <c r="F3">
-        <f t="shared" ca="1" si="0"/>
-        <v>102079.08902664635</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>43755</v>
+      </c>
+      <c r="G3">
+        <v>106186.41</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J66" si="0">"INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES ("&amp;B3&amp;",'"&amp;C3&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;","&amp;G3&amp;");"</f>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101001,'Floating','Personal',36,106186.41);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -477,7 +506,7 @@
         <v>101002</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -485,12 +514,18 @@
       <c r="E4">
         <v>108</v>
       </c>
-      <c r="F4">
-        <f t="shared" ca="1" si="0"/>
-        <v>108244.81509102316</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="2">
+        <v>43974</v>
+      </c>
+      <c r="G4">
+        <v>103241.86</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101002,'Fixed','Housing',108,103241.86);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -498,7 +533,7 @@
         <v>101003</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -506,12 +541,18 @@
       <c r="E5">
         <v>60</v>
       </c>
-      <c r="F5">
-        <f t="shared" ca="1" si="0"/>
-        <v>105522.37545633598</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2">
+        <v>43715</v>
+      </c>
+      <c r="G5">
+        <v>108497.85</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101003,'Floating','Corporate',60,108497.85);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -519,7 +560,7 @@
         <v>101004</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -527,12 +568,18 @@
       <c r="E6">
         <v>96</v>
       </c>
-      <c r="F6">
-        <f t="shared" ca="1" si="0"/>
-        <v>109016.83147824937</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <v>43703</v>
+      </c>
+      <c r="G6">
+        <v>103118.38</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101004,'Fixed','Housing',96,103118.38);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -540,7 +587,7 @@
         <v>101005</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -548,12 +595,18 @@
       <c r="E7">
         <v>48</v>
       </c>
-      <c r="F7">
-        <f t="shared" ca="1" si="0"/>
-        <v>102848.59634735357</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="2">
+        <v>43062</v>
+      </c>
+      <c r="G7">
+        <v>107623.58</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101005,'Floating','Corporate',48,107623.58);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -561,7 +614,7 @@
         <v>101006</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -569,12 +622,18 @@
       <c r="E8">
         <v>48</v>
       </c>
-      <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>105537.13461642376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="2">
+        <v>43470</v>
+      </c>
+      <c r="G8">
+        <v>108034.23</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101006,'Floating','Corporate',48,108034.23);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -582,7 +641,7 @@
         <v>101007</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -590,12 +649,18 @@
       <c r="E9">
         <v>24</v>
       </c>
-      <c r="F9">
-        <f t="shared" ca="1" si="0"/>
-        <v>108035.45890791912</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="2">
+        <v>43659</v>
+      </c>
+      <c r="G9">
+        <v>107279.98</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101007,'Floating','Automobile',24,107279.98);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -603,7 +668,7 @@
         <v>101008</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -611,12 +676,18 @@
       <c r="E10">
         <v>96</v>
       </c>
-      <c r="F10">
-        <f t="shared" ca="1" si="0"/>
-        <v>109089.58384490067</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="2">
+        <v>43457</v>
+      </c>
+      <c r="G10">
+        <v>104016.36</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101008,'Fixed','Automobile',96,104016.36);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -624,7 +695,7 @@
         <v>101009</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -632,12 +703,18 @@
       <c r="E11">
         <v>72</v>
       </c>
-      <c r="F11">
-        <f t="shared" ca="1" si="0"/>
-        <v>109482.21682754304</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="2">
+        <v>44140</v>
+      </c>
+      <c r="G11">
+        <v>108186.79</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101009,'Floating','Automobile',72,108186.79);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -645,7 +722,7 @@
         <v>101010</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -653,12 +730,18 @@
       <c r="E12">
         <v>108</v>
       </c>
-      <c r="F12">
-        <f t="shared" ca="1" si="0"/>
-        <v>100016.23241911929</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="2">
+        <v>43231</v>
+      </c>
+      <c r="G12">
+        <v>103605.8</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101010,'Floating','Automobile',108,103605.8);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -666,7 +749,7 @@
         <v>101011</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -674,12 +757,18 @@
       <c r="E13">
         <v>60</v>
       </c>
-      <c r="F13">
-        <f t="shared" ca="1" si="0"/>
-        <v>100201.74720685424</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="2">
+        <v>42749</v>
+      </c>
+      <c r="G13">
+        <v>104146.81</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101011,'Floating','Automobile',60,104146.81);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -687,7 +776,7 @@
         <v>101012</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -695,12 +784,18 @@
       <c r="E14">
         <v>24</v>
       </c>
-      <c r="F14">
-        <f t="shared" ca="1" si="0"/>
-        <v>101246.20337465421</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="2">
+        <v>42832</v>
+      </c>
+      <c r="G14">
+        <v>104801.5</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101012,'Fixed','Automobile',24,104801.5);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -708,20 +803,26 @@
         <v>101013</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>24</v>
       </c>
-      <c r="F15">
-        <f t="shared" ca="1" si="0"/>
-        <v>107436.74214895791</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="2">
+        <v>43130</v>
+      </c>
+      <c r="G15">
+        <v>101783.86</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101013,'Fixed','Automobile',24,101783.86);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -729,7 +830,7 @@
         <v>101014</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -737,12 +838,18 @@
       <c r="E16">
         <v>96</v>
       </c>
-      <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>103416.12198686252</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="2">
+        <v>43261</v>
+      </c>
+      <c r="G16">
+        <v>109873.03</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101014,'Floating','Corporate',96,109873.03);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -750,7 +857,7 @@
         <v>101015</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -758,12 +865,18 @@
       <c r="E17">
         <v>60</v>
       </c>
-      <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>108000.06281747465</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="2">
+        <v>44141</v>
+      </c>
+      <c r="G17">
+        <v>107099.99</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101015,'Floating','Automobile',60,107099.99);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -771,7 +884,7 @@
         <v>101016</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -779,12 +892,18 @@
       <c r="E18">
         <v>36</v>
       </c>
-      <c r="F18">
-        <f t="shared" ca="1" si="0"/>
-        <v>104752.71509658308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="2">
+        <v>43194</v>
+      </c>
+      <c r="G18">
+        <v>106380.75</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101016,'Floating','Automobile',36,106380.75);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -792,7 +911,7 @@
         <v>101017</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -800,12 +919,18 @@
       <c r="E19">
         <v>72</v>
       </c>
-      <c r="F19">
-        <f t="shared" ca="1" si="0"/>
-        <v>106826.73510219039</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="2">
+        <v>42532</v>
+      </c>
+      <c r="G19">
+        <v>102153.62</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101017,'Floating','Automobile',72,102153.62);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -813,7 +938,7 @@
         <v>101018</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -821,12 +946,18 @@
       <c r="E20">
         <v>36</v>
       </c>
-      <c r="F20">
-        <f t="shared" ca="1" si="0"/>
-        <v>102648.17212329966</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="2">
+        <v>42664</v>
+      </c>
+      <c r="G20">
+        <v>103922.58</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101018,'Fixed','Automobile',36,103922.58);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -834,7 +965,7 @@
         <v>101019</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -842,12 +973,18 @@
       <c r="E21">
         <v>24</v>
       </c>
-      <c r="F21">
-        <f t="shared" ca="1" si="0"/>
-        <v>106837.49854854013</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="2">
+        <v>43972</v>
+      </c>
+      <c r="G21">
+        <v>102673.53</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101019,'Floating','Automobile',24,102673.53);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -855,7 +992,7 @@
         <v>101020</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -863,12 +1000,18 @@
       <c r="E22">
         <v>48</v>
       </c>
-      <c r="F22">
-        <f t="shared" ca="1" si="0"/>
-        <v>105963.11560728161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="2">
+        <v>43963</v>
+      </c>
+      <c r="G22">
+        <v>106168.67</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101020,'Floating','Automobile',48,106168.67);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -876,7 +1019,7 @@
         <v>101021</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -884,12 +1027,18 @@
       <c r="E23">
         <v>72</v>
       </c>
-      <c r="F23">
-        <f t="shared" ca="1" si="0"/>
-        <v>105070.62008283482</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="2">
+        <v>43454</v>
+      </c>
+      <c r="G23">
+        <v>100320.68</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101021,'Floating','Automobile',72,100320.68);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -897,20 +1046,26 @@
         <v>101022</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24">
         <v>36</v>
       </c>
-      <c r="F24">
-        <f t="shared" ca="1" si="0"/>
-        <v>108774.17407700012</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="2">
+        <v>43419</v>
+      </c>
+      <c r="G24">
+        <v>107277.97</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101022,'Floating','Corporate',36,107277.97);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -918,20 +1073,26 @@
         <v>101023</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E25">
         <v>120</v>
       </c>
-      <c r="F25">
-        <f t="shared" ca="1" si="0"/>
-        <v>100662.87802950136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="2">
+        <v>42432</v>
+      </c>
+      <c r="G25">
+        <v>107509.28</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101023,'Fixed','Automobile',120,107509.28);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -939,20 +1100,26 @@
         <v>101024</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E26">
         <v>24</v>
       </c>
-      <c r="F26">
-        <f t="shared" ca="1" si="0"/>
-        <v>105814.12763389667</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="2">
+        <v>44025</v>
+      </c>
+      <c r="G26">
+        <v>104686.2</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101024,'Fixed','Housing',24,104686.2);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -960,7 +1127,7 @@
         <v>101025</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
@@ -968,12 +1135,18 @@
       <c r="E27">
         <v>96</v>
       </c>
-      <c r="F27">
-        <f t="shared" ca="1" si="0"/>
-        <v>102150.59835961617</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="2">
+        <v>43093</v>
+      </c>
+      <c r="G27">
+        <v>101053.2</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101025,'Fixed','Corporate',96,101053.2);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -981,20 +1154,26 @@
         <v>101026</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28">
         <v>24</v>
       </c>
-      <c r="F28">
-        <f t="shared" ca="1" si="0"/>
-        <v>108726.87985148098</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="2">
+        <v>43158</v>
+      </c>
+      <c r="G28">
+        <v>100840.78</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101026,'Fixed','Corporate',24,100840.78);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1002,7 +1181,7 @@
         <v>101027</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -1010,12 +1189,18 @@
       <c r="E29">
         <v>84</v>
       </c>
-      <c r="F29">
-        <f t="shared" ca="1" si="0"/>
-        <v>104158.11824329584</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="2">
+        <v>42406</v>
+      </c>
+      <c r="G29">
+        <v>109769.46</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101027,'Fixed','Personal',84,109769.46);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1023,20 +1208,26 @@
         <v>101028</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E30">
         <v>60</v>
       </c>
-      <c r="F30">
-        <f t="shared" ca="1" si="0"/>
-        <v>104749.6772704974</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="2">
+        <v>42613</v>
+      </c>
+      <c r="G30">
+        <v>101720.88</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101028,'Fixed','Housing',60,101720.88);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1044,20 +1235,26 @@
         <v>101029</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E31">
         <v>96</v>
       </c>
-      <c r="F31">
-        <f t="shared" ca="1" si="0"/>
-        <v>104204.15439447812</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="2">
+        <v>42464</v>
+      </c>
+      <c r="G31">
+        <v>107303.03999999999</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101029,'Fixed','Automobile',96,107303.04);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1065,20 +1262,26 @@
         <v>101030</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E32">
         <v>72</v>
       </c>
-      <c r="F32">
-        <f t="shared" ca="1" si="0"/>
-        <v>107096.40764402389</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="2">
+        <v>42975</v>
+      </c>
+      <c r="G32">
+        <v>103492.6</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101030,'Floating','Corporate',72,103492.6);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1086,7 +1289,7 @@
         <v>101031</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -1094,12 +1297,18 @@
       <c r="E33">
         <v>48</v>
       </c>
-      <c r="F33">
-        <f t="shared" ca="1" si="0"/>
-        <v>106739.20745386899</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="2">
+        <v>43886</v>
+      </c>
+      <c r="G33">
+        <v>105505.91</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101031,'Floating','Personal',48,105505.91);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1107,7 +1316,7 @@
         <v>101032</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -1115,12 +1324,18 @@
       <c r="E34">
         <v>84</v>
       </c>
-      <c r="F34">
-        <f t="shared" ca="1" si="0"/>
-        <v>109708.66258931653</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="2">
+        <v>43121</v>
+      </c>
+      <c r="G34">
+        <v>100660.62</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101032,'Floating','Corporate',84,100660.62);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1128,7 +1343,7 @@
         <v>101033</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -1136,12 +1351,18 @@
       <c r="E35">
         <v>12</v>
       </c>
-      <c r="F35">
-        <f t="shared" ca="1" si="0"/>
-        <v>103561.98794467103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="2">
+        <v>42497</v>
+      </c>
+      <c r="G35">
+        <v>104137.47</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101033,'Fixed','Housing',12,104137.47);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1149,7 +1370,7 @@
         <v>101034</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -1157,12 +1378,18 @@
       <c r="E36">
         <v>108</v>
       </c>
-      <c r="F36">
-        <f t="shared" ca="1" si="0"/>
-        <v>100600.79025134021</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="2">
+        <v>44162</v>
+      </c>
+      <c r="G36">
+        <v>109406.89</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101034,'Floating','Automobile',108,109406.89);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1170,7 +1397,7 @@
         <v>101035</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
@@ -1178,12 +1405,18 @@
       <c r="E37">
         <v>24</v>
       </c>
-      <c r="F37">
-        <f t="shared" ca="1" si="0"/>
-        <v>101951.34731546798</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="2">
+        <v>43014</v>
+      </c>
+      <c r="G37">
+        <v>100321.31</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101035,'Floating','Personal',24,100321.31);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1191,7 +1424,7 @@
         <v>101036</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
@@ -1199,12 +1432,18 @@
       <c r="E38">
         <v>108</v>
       </c>
-      <c r="F38">
-        <f t="shared" ca="1" si="0"/>
-        <v>103423.78960243917</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="2">
+        <v>42552</v>
+      </c>
+      <c r="G38">
+        <v>102803.42</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101036,'Fixed','Corporate',108,102803.42);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1212,7 +1451,7 @@
         <v>101037</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
@@ -1220,12 +1459,18 @@
       <c r="E39">
         <v>48</v>
       </c>
-      <c r="F39">
-        <f t="shared" ca="1" si="0"/>
-        <v>100510.11838472764</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="2">
+        <v>43079</v>
+      </c>
+      <c r="G39">
+        <v>100140.72</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101037,'Fixed','Housing',48,100140.72);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1233,7 +1478,7 @@
         <v>101038</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -1241,12 +1486,18 @@
       <c r="E40">
         <v>96</v>
       </c>
-      <c r="F40">
-        <f t="shared" ca="1" si="0"/>
-        <v>109249.79538887971</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="2">
+        <v>43665</v>
+      </c>
+      <c r="G40">
+        <v>103348.43</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101038,'Floating','Personal',96,103348.43);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1254,20 +1505,26 @@
         <v>101039</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E41">
         <v>36</v>
       </c>
-      <c r="F41">
-        <f t="shared" ca="1" si="0"/>
-        <v>100709.57338407355</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="2">
+        <v>43193</v>
+      </c>
+      <c r="G41">
+        <v>106750.75</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101039,'Fixed','Housing',36,106750.75);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1275,7 +1532,7 @@
         <v>101040</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
@@ -1283,12 +1540,18 @@
       <c r="E42">
         <v>24</v>
       </c>
-      <c r="F42">
-        <f t="shared" ca="1" si="0"/>
-        <v>105512.2444905126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="2">
+        <v>42736</v>
+      </c>
+      <c r="G42">
+        <v>109316.05</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101040,'Fixed','Housing',24,109316.05);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1296,7 +1559,7 @@
         <v>101041</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
@@ -1304,12 +1567,18 @@
       <c r="E43">
         <v>72</v>
       </c>
-      <c r="F43">
-        <f t="shared" ca="1" si="0"/>
-        <v>108657.98995731046</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="2">
+        <v>43600</v>
+      </c>
+      <c r="G43">
+        <v>101799.58</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101041,'Fixed','Corporate',72,101799.58);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1317,7 +1586,7 @@
         <v>101042</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -1325,12 +1594,18 @@
       <c r="E44">
         <v>108</v>
       </c>
-      <c r="F44">
-        <f t="shared" ca="1" si="0"/>
-        <v>106625.542896642</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="2">
+        <v>42603</v>
+      </c>
+      <c r="G44">
+        <v>103276.04</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101042,'Fixed','Automobile',108,103276.04);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1338,20 +1613,26 @@
         <v>101043</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E45">
         <v>36</v>
       </c>
-      <c r="F45">
-        <f t="shared" ca="1" si="0"/>
-        <v>107712.07568749826</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="2">
+        <v>43153</v>
+      </c>
+      <c r="G45">
+        <v>101766.24</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101043,'Fixed','Housing',36,101766.24);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1359,7 +1640,7 @@
         <v>101044</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
@@ -1367,12 +1648,18 @@
       <c r="E46">
         <v>60</v>
       </c>
-      <c r="F46">
-        <f t="shared" ca="1" si="0"/>
-        <v>107514.26611389199</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="2">
+        <v>44099</v>
+      </c>
+      <c r="G46">
+        <v>109361.77</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101044,'Floating','Personal',60,109361.77);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1380,7 +1667,7 @@
         <v>101045</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
         <v>5</v>
@@ -1388,12 +1675,18 @@
       <c r="E47">
         <v>12</v>
       </c>
-      <c r="F47">
-        <f t="shared" ca="1" si="0"/>
-        <v>101673.67585924552</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="2">
+        <v>43843</v>
+      </c>
+      <c r="G47">
+        <v>101037.09</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101045,'Floating','Housing',12,101037.09);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1401,7 +1694,7 @@
         <v>101046</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
         <v>8</v>
@@ -1409,12 +1702,18 @@
       <c r="E48">
         <v>72</v>
       </c>
-      <c r="F48">
-        <f t="shared" ca="1" si="0"/>
-        <v>105595.64937469557</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="2">
+        <v>42648</v>
+      </c>
+      <c r="G48">
+        <v>100490.43</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101046,'Floating','Corporate',72,100490.43);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1422,7 +1721,7 @@
         <v>101047</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
@@ -1430,12 +1729,18 @@
       <c r="E49">
         <v>84</v>
       </c>
-      <c r="F49">
-        <f t="shared" ca="1" si="0"/>
-        <v>102009.24423969905</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="2">
+        <v>43913</v>
+      </c>
+      <c r="G49">
+        <v>100409.03</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101047,'Floating','Automobile',84,100409.03);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1443,7 +1748,7 @@
         <v>101048</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
@@ -1451,12 +1756,18 @@
       <c r="E50">
         <v>72</v>
       </c>
-      <c r="F50">
-        <f t="shared" ca="1" si="0"/>
-        <v>108516.08329848658</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="2">
+        <v>44192</v>
+      </c>
+      <c r="G50">
+        <v>106591.49</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101048,'Floating','Corporate',72,106591.49);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1464,7 +1775,7 @@
         <v>101049</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D51" t="s">
         <v>5</v>
@@ -1472,12 +1783,18 @@
       <c r="E51">
         <v>60</v>
       </c>
-      <c r="F51">
-        <f t="shared" ca="1" si="0"/>
-        <v>106691.17164008234</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="2">
+        <v>43848</v>
+      </c>
+      <c r="G51">
+        <v>108942.56</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101049,'Fixed','Housing',60,108942.56);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1485,7 +1802,7 @@
         <v>101050</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -1493,12 +1810,18 @@
       <c r="E52">
         <v>108</v>
       </c>
-      <c r="F52">
-        <f t="shared" ca="1" si="0"/>
-        <v>106217.32728193272</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="2">
+        <v>43155</v>
+      </c>
+      <c r="G52">
+        <v>106577.48</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101050,'Floating','Personal',108,106577.48);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1506,20 +1829,26 @@
         <v>101051</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E53">
         <v>120</v>
       </c>
-      <c r="F53">
-        <f t="shared" ca="1" si="0"/>
-        <v>100795.78679337833</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="2">
+        <v>43207</v>
+      </c>
+      <c r="G53">
+        <v>104373.35</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101051,'Floating','Housing',120,104373.35);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1527,7 +1856,7 @@
         <v>101052</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D54" t="s">
         <v>8</v>
@@ -1535,12 +1864,18 @@
       <c r="E54">
         <v>84</v>
       </c>
-      <c r="F54">
-        <f t="shared" ca="1" si="0"/>
-        <v>103322.39994432553</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="2">
+        <v>44161</v>
+      </c>
+      <c r="G54">
+        <v>104546.7</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101052,'Fixed','Corporate',84,104546.7);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1548,20 +1883,26 @@
         <v>101053</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E55">
         <v>108</v>
       </c>
-      <c r="F55">
-        <f t="shared" ca="1" si="0"/>
-        <v>109674.53110924862</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="2">
+        <v>43444</v>
+      </c>
+      <c r="G55">
+        <v>106114.48</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101053,'Fixed','Personal',108,106114.48);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1569,7 +1910,7 @@
         <v>101054</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
@@ -1577,12 +1918,18 @@
       <c r="E56">
         <v>72</v>
       </c>
-      <c r="F56">
-        <f t="shared" ca="1" si="0"/>
-        <v>108326.12060568924</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="2">
+        <v>42376</v>
+      </c>
+      <c r="G56">
+        <v>108335.42</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101054,'Fixed','Automobile',72,108335.42);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1590,7 +1937,7 @@
         <v>101055</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -1598,12 +1945,18 @@
       <c r="E57">
         <v>72</v>
       </c>
-      <c r="F57">
-        <f t="shared" ca="1" si="0"/>
-        <v>107266.62211671501</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="2">
+        <v>42523</v>
+      </c>
+      <c r="G57">
+        <v>101854.94</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101055,'Floating','Personal',72,101854.94);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1611,20 +1964,26 @@
         <v>101056</v>
       </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E58">
         <v>120</v>
       </c>
-      <c r="F58">
-        <f t="shared" ca="1" si="0"/>
-        <v>109229.40378016199</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="2">
+        <v>42641</v>
+      </c>
+      <c r="G58">
+        <v>108640.49</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101056,'Fixed','Personal',120,108640.49);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1632,7 +1991,7 @@
         <v>101057</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
@@ -1640,12 +1999,18 @@
       <c r="E59">
         <v>72</v>
       </c>
-      <c r="F59">
-        <f t="shared" ca="1" si="0"/>
-        <v>104985.25355583071</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="2">
+        <v>43009</v>
+      </c>
+      <c r="G59">
+        <v>101375.16</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101057,'Fixed','Corporate',72,101375.16);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1653,20 +2018,26 @@
         <v>101058</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E60">
         <v>36</v>
       </c>
-      <c r="F60">
-        <f t="shared" ca="1" si="0"/>
-        <v>106723.69285228233</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="2">
+        <v>43705</v>
+      </c>
+      <c r="G60">
+        <v>100644.47</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101058,'Floating','Personal',36,100644.47);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1674,20 +2045,26 @@
         <v>101059</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E61">
         <v>84</v>
       </c>
-      <c r="F61">
-        <f t="shared" ca="1" si="0"/>
-        <v>108621.26379276733</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="2">
+        <v>43374</v>
+      </c>
+      <c r="G61">
+        <v>106058.61</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101059,'Fixed','Personal',84,106058.61);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1695,7 +2072,7 @@
         <v>101060</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -1703,12 +2080,18 @@
       <c r="E62">
         <v>120</v>
       </c>
-      <c r="F62">
-        <f t="shared" ca="1" si="0"/>
-        <v>105422.39072150957</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="2">
+        <v>43867</v>
+      </c>
+      <c r="G62">
+        <v>103099.78</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101060,'Floating','Personal',120,103099.78);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1716,20 +2099,26 @@
         <v>101061</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E63">
         <v>72</v>
       </c>
-      <c r="F63">
-        <f t="shared" ca="1" si="0"/>
-        <v>102702.49302710887</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="2">
+        <v>43647</v>
+      </c>
+      <c r="G63">
+        <v>103597.6</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101061,'Fixed','Personal',72,103597.6);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1737,7 +2126,7 @@
         <v>101062</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D64" t="s">
         <v>5</v>
@@ -1745,12 +2134,18 @@
       <c r="E64">
         <v>24</v>
       </c>
-      <c r="F64">
-        <f t="shared" ca="1" si="0"/>
-        <v>105316.25701128122</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="2">
+        <v>43025</v>
+      </c>
+      <c r="G64">
+        <v>106984.42</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101062,'Fixed','Housing',24,106984.42);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1758,7 +2153,7 @@
         <v>101063</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -1766,12 +2161,18 @@
       <c r="E65">
         <v>120</v>
       </c>
-      <c r="F65">
-        <f t="shared" ca="1" si="0"/>
-        <v>106280.44946080376</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="2">
+        <v>43760</v>
+      </c>
+      <c r="G65">
+        <v>104494.34</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101063,'Floating','Personal',120,104494.34);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1779,7 +2180,7 @@
         <v>101064</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D66" t="s">
         <v>8</v>
@@ -1787,12 +2188,18 @@
       <c r="E66">
         <v>84</v>
       </c>
-      <c r="F66">
-        <f t="shared" ref="F66:F101" ca="1" si="1">RAND()*10000 + 100000</f>
-        <v>102654.94066586836</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="2">
+        <v>43727</v>
+      </c>
+      <c r="G66">
+        <v>109574.39</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101064,'Fixed','Corporate',84,109574.39);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1800,7 +2207,7 @@
         <v>101065</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D67" t="s">
         <v>8</v>
@@ -1808,12 +2215,18 @@
       <c r="E67">
         <v>36</v>
       </c>
-      <c r="F67">
-        <f t="shared" ca="1" si="1"/>
-        <v>107254.55756904483</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="2">
+        <v>44114</v>
+      </c>
+      <c r="G67">
+        <v>102145.65</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J101" si="1">"INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES ("&amp;B67&amp;",'"&amp;C67&amp;"','"&amp;D67&amp;"',"&amp;E67&amp;","&amp;G67&amp;");"</f>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101065,'Floating','Corporate',36,102145.65);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1821,7 +2234,7 @@
         <v>101066</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
@@ -1829,12 +2242,18 @@
       <c r="E68">
         <v>72</v>
       </c>
-      <c r="F68">
-        <f t="shared" ca="1" si="1"/>
-        <v>105273.6061833174</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="2">
+        <v>43929</v>
+      </c>
+      <c r="G68">
+        <v>100094.01</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101066,'Fixed','Automobile',72,100094.01);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1842,7 +2261,7 @@
         <v>101067</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D69" t="s">
         <v>5</v>
@@ -1850,12 +2269,18 @@
       <c r="E69">
         <v>120</v>
       </c>
-      <c r="F69">
-        <f t="shared" ca="1" si="1"/>
-        <v>104295.55655459975</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F69" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G69">
+        <v>101688.94</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101067,'Floating','Housing',120,101688.94);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1863,7 +2288,7 @@
         <v>101068</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s">
         <v>5</v>
@@ -1871,12 +2296,18 @@
       <c r="E70">
         <v>72</v>
       </c>
-      <c r="F70">
-        <f t="shared" ca="1" si="1"/>
-        <v>101541.10859786773</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F70" s="2">
+        <v>42779</v>
+      </c>
+      <c r="G70">
+        <v>109803.75</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101068,'Floating','Housing',72,109803.75);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1884,7 +2315,7 @@
         <v>101069</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
         <v>6</v>
@@ -1892,12 +2323,18 @@
       <c r="E71">
         <v>96</v>
       </c>
-      <c r="F71">
-        <f t="shared" ca="1" si="1"/>
-        <v>108408.19511954809</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F71" s="2">
+        <v>43634</v>
+      </c>
+      <c r="G71">
+        <v>106954.79</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101069,'Floating','Automobile',96,106954.79);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1905,7 +2342,7 @@
         <v>101070</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D72" t="s">
         <v>8</v>
@@ -1913,12 +2350,18 @@
       <c r="E72">
         <v>60</v>
       </c>
-      <c r="F72">
-        <f t="shared" ca="1" si="1"/>
-        <v>104280.00669278835</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F72" s="2">
+        <v>43959</v>
+      </c>
+      <c r="G72">
+        <v>109732.55</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101070,'Fixed','Corporate',60,109732.55);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1926,7 +2369,7 @@
         <v>101071</v>
       </c>
       <c r="C73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D73" t="s">
         <v>6</v>
@@ -1934,12 +2377,18 @@
       <c r="E73">
         <v>24</v>
       </c>
-      <c r="F73">
-        <f t="shared" ca="1" si="1"/>
-        <v>109424.64411022625</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="2">
+        <v>43888</v>
+      </c>
+      <c r="G73">
+        <v>109962.04</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101071,'Floating','Automobile',24,109962.04);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1947,7 +2396,7 @@
         <v>101072</v>
       </c>
       <c r="C74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D74" t="s">
         <v>6</v>
@@ -1955,12 +2404,18 @@
       <c r="E74">
         <v>84</v>
       </c>
-      <c r="F74">
-        <f t="shared" ca="1" si="1"/>
-        <v>106627.96018370293</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="2">
+        <v>44066</v>
+      </c>
+      <c r="G74">
+        <v>100801.69</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101072,'Fixed','Automobile',84,100801.69);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1968,20 +2423,26 @@
         <v>101073</v>
       </c>
       <c r="C75" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E75">
         <v>108</v>
       </c>
-      <c r="F75">
-        <f t="shared" ca="1" si="1"/>
-        <v>104408.33035440939</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="2">
+        <v>43129</v>
+      </c>
+      <c r="G75">
+        <v>106815.22</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101073,'Floating','Personal',108,106815.22);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1989,7 +2450,7 @@
         <v>101074</v>
       </c>
       <c r="C76" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
@@ -1997,12 +2458,18 @@
       <c r="E76">
         <v>96</v>
       </c>
-      <c r="F76">
-        <f t="shared" ca="1" si="1"/>
-        <v>109518.66507228847</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="2">
+        <v>43608</v>
+      </c>
+      <c r="G76">
+        <v>103272.78</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101074,'Floating','Corporate',96,103272.78);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2010,7 +2477,7 @@
         <v>101075</v>
       </c>
       <c r="C77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D77" t="s">
         <v>6</v>
@@ -2018,12 +2485,18 @@
       <c r="E77">
         <v>36</v>
       </c>
-      <c r="F77">
-        <f t="shared" ca="1" si="1"/>
-        <v>102064.54663482001</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="2">
+        <v>43442</v>
+      </c>
+      <c r="G77">
+        <v>102302.67</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101075,'Fixed','Automobile',36,102302.67);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2031,7 +2504,7 @@
         <v>101076</v>
       </c>
       <c r="C78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D78" t="s">
         <v>5</v>
@@ -2039,12 +2512,18 @@
       <c r="E78">
         <v>60</v>
       </c>
-      <c r="F78">
-        <f t="shared" ca="1" si="1"/>
-        <v>109960.76386424272</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="2">
+        <v>43075</v>
+      </c>
+      <c r="G78">
+        <v>108049.06</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101076,'Floating','Housing',60,108049.06);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2052,20 +2531,26 @@
         <v>101077</v>
       </c>
       <c r="C79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E79">
         <v>108</v>
       </c>
-      <c r="F79">
-        <f t="shared" ca="1" si="1"/>
-        <v>107515.46581667595</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="2">
+        <v>42604</v>
+      </c>
+      <c r="G79">
+        <v>104264.53</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101077,'Fixed','Personal',108,104264.53);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2073,7 +2558,7 @@
         <v>101078</v>
       </c>
       <c r="C80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D80" t="s">
         <v>8</v>
@@ -2081,12 +2566,18 @@
       <c r="E80">
         <v>24</v>
       </c>
-      <c r="F80">
-        <f t="shared" ca="1" si="1"/>
-        <v>105300.84649914684</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F80" s="2">
+        <v>43474</v>
+      </c>
+      <c r="G80">
+        <v>109014.52</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101078,'Floating','Corporate',24,109014.52);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2094,7 +2585,7 @@
         <v>101079</v>
       </c>
       <c r="C81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D81" t="s">
         <v>6</v>
@@ -2102,12 +2593,18 @@
       <c r="E81">
         <v>120</v>
       </c>
-      <c r="F81">
-        <f t="shared" ca="1" si="1"/>
-        <v>106076.1440820385</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="2">
+        <v>42479</v>
+      </c>
+      <c r="G81">
+        <v>106847.31</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101079,'Fixed','Automobile',120,106847.31);</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2115,7 +2612,7 @@
         <v>101080</v>
       </c>
       <c r="C82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
@@ -2123,12 +2620,18 @@
       <c r="E82">
         <v>72</v>
       </c>
-      <c r="F82">
-        <f t="shared" ca="1" si="1"/>
-        <v>100054.98776560358</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="2">
+        <v>44027</v>
+      </c>
+      <c r="G82">
+        <v>108345.84</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101080,'Fixed','Personal',72,108345.84);</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2136,20 +2639,26 @@
         <v>101081</v>
       </c>
       <c r="C83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D83" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E83">
         <v>96</v>
       </c>
-      <c r="F83">
-        <f t="shared" ca="1" si="1"/>
-        <v>100812.9606168164</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="2">
+        <v>43074</v>
+      </c>
+      <c r="G83">
+        <v>103573.7</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101081,'Fixed','Personal',96,103573.7);</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2157,20 +2666,26 @@
         <v>101082</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D84" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E84">
         <v>120</v>
       </c>
-      <c r="F84">
-        <f t="shared" ca="1" si="1"/>
-        <v>103455.78064640186</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="2">
+        <v>43903</v>
+      </c>
+      <c r="G84">
+        <v>103728.24</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101082,'Floating','Personal',120,103728.24);</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2178,20 +2693,26 @@
         <v>101083</v>
       </c>
       <c r="C85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E85">
         <v>96</v>
       </c>
-      <c r="F85">
-        <f t="shared" ca="1" si="1"/>
-        <v>101810.44500452638</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="2">
+        <v>42508</v>
+      </c>
+      <c r="G85">
+        <v>108264.33</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101083,'Fixed','Personal',96,108264.33);</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2199,7 +2720,7 @@
         <v>101084</v>
       </c>
       <c r="C86" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D86" t="s">
         <v>7</v>
@@ -2207,12 +2728,18 @@
       <c r="E86">
         <v>36</v>
       </c>
-      <c r="F86">
-        <f t="shared" ca="1" si="1"/>
-        <v>101700.59513004062</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="2">
+        <v>43578</v>
+      </c>
+      <c r="G86">
+        <v>100255.65</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101084,'Floating','Personal',36,100255.65);</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2220,7 +2747,7 @@
         <v>101085</v>
       </c>
       <c r="C87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
@@ -2228,12 +2755,18 @@
       <c r="E87">
         <v>12</v>
       </c>
-      <c r="F87">
-        <f t="shared" ca="1" si="1"/>
-        <v>108063.87097214852</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="2">
+        <v>44025</v>
+      </c>
+      <c r="G87">
+        <v>105091.82</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101085,'Fixed','Automobile',12,105091.82);</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2241,7 +2774,7 @@
         <v>101086</v>
       </c>
       <c r="C88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
@@ -2249,12 +2782,18 @@
       <c r="E88">
         <v>12</v>
       </c>
-      <c r="F88">
-        <f t="shared" ca="1" si="1"/>
-        <v>102187.05241860947</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="2">
+        <v>43739</v>
+      </c>
+      <c r="G88">
+        <v>105973.29</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101086,'Fixed','Automobile',12,105973.29);</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2262,7 +2801,7 @@
         <v>101087</v>
       </c>
       <c r="C89" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D89" t="s">
         <v>7</v>
@@ -2270,12 +2809,18 @@
       <c r="E89">
         <v>84</v>
       </c>
-      <c r="F89">
-        <f t="shared" ca="1" si="1"/>
-        <v>104844.53447599988</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="2">
+        <v>43045</v>
+      </c>
+      <c r="G89">
+        <v>103021.48</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101087,'Floating','Personal',84,103021.48);</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2283,20 +2828,26 @@
         <v>101088</v>
       </c>
       <c r="C90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D90" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E90">
         <v>108</v>
       </c>
-      <c r="F90">
-        <f t="shared" ca="1" si="1"/>
-        <v>104402.78194990949</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="2">
+        <v>43056</v>
+      </c>
+      <c r="G90">
+        <v>101881.74</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101088,'Fixed','Personal',108,101881.74);</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2304,7 +2855,7 @@
         <v>101089</v>
       </c>
       <c r="C91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D91" t="s">
         <v>5</v>
@@ -2312,12 +2863,18 @@
       <c r="E91">
         <v>120</v>
       </c>
-      <c r="F91">
-        <f t="shared" ca="1" si="1"/>
-        <v>103186.96266244247</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="2">
+        <v>42421</v>
+      </c>
+      <c r="G91">
+        <v>103090.73</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101089,'Fixed','Housing',120,103090.73);</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2325,7 +2882,7 @@
         <v>101090</v>
       </c>
       <c r="C92" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D92" t="s">
         <v>5</v>
@@ -2333,12 +2890,18 @@
       <c r="E92">
         <v>84</v>
       </c>
-      <c r="F92">
-        <f t="shared" ca="1" si="1"/>
-        <v>109295.35795054238</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="2">
+        <v>43863</v>
+      </c>
+      <c r="G92">
+        <v>109677.49</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101090,'Floating','Housing',84,109677.49);</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2346,7 +2909,7 @@
         <v>101091</v>
       </c>
       <c r="C93" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
@@ -2354,12 +2917,18 @@
       <c r="E93">
         <v>12</v>
       </c>
-      <c r="F93">
-        <f t="shared" ca="1" si="1"/>
-        <v>102871.8191780262</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="2">
+        <v>42858</v>
+      </c>
+      <c r="G93">
+        <v>109240.26</v>
+      </c>
+      <c r="J93" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101091,'Floating','Automobile',12,109240.26);</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2367,7 +2936,7 @@
         <v>101092</v>
       </c>
       <c r="C94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D94" t="s">
         <v>5</v>
@@ -2375,12 +2944,18 @@
       <c r="E94">
         <v>24</v>
       </c>
-      <c r="F94">
-        <f t="shared" ca="1" si="1"/>
-        <v>109526.17127410442</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="2">
+        <v>44028</v>
+      </c>
+      <c r="G94">
+        <v>100884.75</v>
+      </c>
+      <c r="J94" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101092,'Fixed','Housing',24,100884.75);</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2388,7 +2963,7 @@
         <v>101093</v>
       </c>
       <c r="C95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
@@ -2396,12 +2971,18 @@
       <c r="E95">
         <v>120</v>
       </c>
-      <c r="F95">
-        <f t="shared" ca="1" si="1"/>
-        <v>106174.50173977591</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="2">
+        <v>42911</v>
+      </c>
+      <c r="G95">
+        <v>103963.68</v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101093,'Fixed','Automobile',120,103963.68);</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2409,7 +2990,7 @@
         <v>101094</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D96" t="s">
         <v>5</v>
@@ -2417,12 +2998,18 @@
       <c r="E96">
         <v>60</v>
       </c>
-      <c r="F96">
-        <f t="shared" ca="1" si="1"/>
-        <v>106285.1279592888</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="2">
+        <v>43446</v>
+      </c>
+      <c r="G96">
+        <v>108976.46</v>
+      </c>
+      <c r="J96" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101094,'Floating','Housing',60,108976.46);</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2430,7 +3017,7 @@
         <v>101095</v>
       </c>
       <c r="C97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D97" t="s">
         <v>5</v>
@@ -2438,12 +3025,18 @@
       <c r="E97">
         <v>24</v>
       </c>
-      <c r="F97">
-        <f t="shared" ca="1" si="1"/>
-        <v>104355.74772843195</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="2">
+        <v>42884</v>
+      </c>
+      <c r="G97">
+        <v>103617.54</v>
+      </c>
+      <c r="J97" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101095,'Fixed','Housing',24,103617.54);</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2451,7 +3044,7 @@
         <v>101096</v>
       </c>
       <c r="C98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D98" t="s">
         <v>7</v>
@@ -2459,12 +3052,18 @@
       <c r="E98">
         <v>120</v>
       </c>
-      <c r="F98">
-        <f t="shared" ca="1" si="1"/>
-        <v>104891.58586412659</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="2">
+        <v>44011</v>
+      </c>
+      <c r="G98">
+        <v>104275.58</v>
+      </c>
+      <c r="J98" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101096,'Fixed','Personal',120,104275.58);</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2472,7 +3071,7 @@
         <v>101097</v>
       </c>
       <c r="C99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D99" t="s">
         <v>8</v>
@@ -2480,12 +3079,18 @@
       <c r="E99">
         <v>36</v>
       </c>
-      <c r="F99">
-        <f t="shared" ca="1" si="1"/>
-        <v>108404.66079424293</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="2">
+        <v>42539</v>
+      </c>
+      <c r="G99">
+        <v>107392.59</v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101097,'Fixed','Corporate',36,107392.59);</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2493,7 +3098,7 @@
         <v>101098</v>
       </c>
       <c r="C100" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D100" t="s">
         <v>5</v>
@@ -2501,12 +3106,18 @@
       <c r="E100">
         <v>48</v>
       </c>
-      <c r="F100">
-        <f t="shared" ca="1" si="1"/>
-        <v>108977.1640167017</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="2">
+        <v>43286</v>
+      </c>
+      <c r="G100">
+        <v>102840.04</v>
+      </c>
+      <c r="J100" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101098,'Floating','Housing',48,102840.04);</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2514,7 +3125,7 @@
         <v>101099</v>
       </c>
       <c r="C101" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D101" t="s">
         <v>5</v>
@@ -2522,12 +3133,19 @@
       <c r="E101">
         <v>120</v>
       </c>
-      <c r="F101">
-        <f t="shared" ca="1" si="1"/>
-        <v>105769.72890772138</v>
+      <c r="F101" s="2">
+        <v>43756</v>
+      </c>
+      <c r="G101">
+        <v>104867.95</v>
+      </c>
+      <c r="J101" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101099,'Floating','Housing',120,104867.95);</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Reduced Loans count to 60
</commit_message>
<xml_diff>
--- a/Dummy Data/Dim_Loans.xlsx
+++ b/Dummy Data/Dim_Loans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sem2\Data Warehousing\assigment\Loan-Data-Warehouse\Dummy Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF35F19-CF4A-4964-AE81-003A6FBA27DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1D731C-C1D2-49B5-9604-6B89C29E7D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3145,7 +3145,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Lineage added to Dim_Loans and shortened excel to 60 loans
</commit_message>
<xml_diff>
--- a/Dummy Data/Dim_Loans.xlsx
+++ b/Dummy Data/Dim_Loans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sem2\Data Warehousing\assigment\Loan-Data-Warehouse\Dummy Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1D731C-C1D2-49B5-9604-6B89C29E7D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9164395-975A-45E0-AE1A-425ABF2C7157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="14">
   <si>
     <t>Loan Key</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Loan Issue date</t>
+  </si>
+  <si>
+    <t>Lineage Key</t>
   </si>
 </sst>
 </file>
@@ -405,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J61" sqref="J2:J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,6 +446,9 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -466,9 +472,12 @@
       <c r="G2">
         <v>106485.57</v>
       </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
       <c r="J2" t="str">
-        <f>"INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES ("&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;","&amp;G2&amp;");"</f>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101000,'Floating','Personal',96,106485.57);</v>
+        <f>"INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES ("&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;","&amp;G2&amp;","&amp;H2&amp;");"</f>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101000,'Floating','Personal',96,106485.57,4);</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -493,9 +502,12 @@
       <c r="G3">
         <v>106186.41</v>
       </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J66" si="0">"INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES ("&amp;B3&amp;",'"&amp;C3&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;","&amp;G3&amp;");"</f>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101001,'Floating','Personal',36,106186.41);</v>
+        <f t="shared" ref="J3:J66" si="0">"INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES ("&amp;B3&amp;",'"&amp;C3&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;","&amp;G3&amp;","&amp;H3&amp;");"</f>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101001,'Floating','Personal',36,106186.41,4);</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -520,9 +532,12 @@
       <c r="G4">
         <v>103241.86</v>
       </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101002,'Fixed','Housing',108,103241.86);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101002,'Fixed','Housing',108,103241.86,4);</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -547,9 +562,12 @@
       <c r="G5">
         <v>108497.85</v>
       </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101003,'Floating','Corporate',60,108497.85);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101003,'Floating','Corporate',60,108497.85,4);</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -574,9 +592,12 @@
       <c r="G6">
         <v>103118.38</v>
       </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101004,'Fixed','Housing',96,103118.38);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101004,'Fixed','Housing',96,103118.38,4);</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -601,9 +622,12 @@
       <c r="G7">
         <v>107623.58</v>
       </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101005,'Floating','Corporate',48,107623.58);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101005,'Floating','Corporate',48,107623.58,4);</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -628,9 +652,12 @@
       <c r="G8">
         <v>108034.23</v>
       </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101006,'Floating','Corporate',48,108034.23);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101006,'Floating','Corporate',48,108034.23,4);</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -655,9 +682,12 @@
       <c r="G9">
         <v>107279.98</v>
       </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101007,'Floating','Automobile',24,107279.98);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101007,'Floating','Automobile',24,107279.98,4);</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -682,9 +712,12 @@
       <c r="G10">
         <v>104016.36</v>
       </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101008,'Fixed','Automobile',96,104016.36);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101008,'Fixed','Automobile',96,104016.36,4);</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -709,9 +742,12 @@
       <c r="G11">
         <v>108186.79</v>
       </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101009,'Floating','Automobile',72,108186.79);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101009,'Floating','Automobile',72,108186.79,4);</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -736,9 +772,12 @@
       <c r="G12">
         <v>103605.8</v>
       </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101010,'Floating','Automobile',108,103605.8);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101010,'Floating','Automobile',108,103605.8,4);</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -763,9 +802,12 @@
       <c r="G13">
         <v>104146.81</v>
       </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101011,'Floating','Automobile',60,104146.81);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101011,'Floating','Automobile',60,104146.81,4);</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -790,9 +832,12 @@
       <c r="G14">
         <v>104801.5</v>
       </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101012,'Fixed','Automobile',24,104801.5);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101012,'Fixed','Automobile',24,104801.5,4);</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -817,9 +862,12 @@
       <c r="G15">
         <v>101783.86</v>
       </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101013,'Fixed','Automobile',24,101783.86);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101013,'Fixed','Automobile',24,101783.86,4);</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -844,9 +892,12 @@
       <c r="G16">
         <v>109873.03</v>
       </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101014,'Floating','Corporate',96,109873.03);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101014,'Floating','Corporate',96,109873.03,4);</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -871,9 +922,12 @@
       <c r="G17">
         <v>107099.99</v>
       </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101015,'Floating','Automobile',60,107099.99);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101015,'Floating','Automobile',60,107099.99,4);</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -898,9 +952,12 @@
       <c r="G18">
         <v>106380.75</v>
       </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101016,'Floating','Automobile',36,106380.75);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101016,'Floating','Automobile',36,106380.75,4);</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -925,9 +982,12 @@
       <c r="G19">
         <v>102153.62</v>
       </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101017,'Floating','Automobile',72,102153.62);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101017,'Floating','Automobile',72,102153.62,4);</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -952,9 +1012,12 @@
       <c r="G20">
         <v>103922.58</v>
       </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101018,'Fixed','Automobile',36,103922.58);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101018,'Fixed','Automobile',36,103922.58,4);</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -979,9 +1042,12 @@
       <c r="G21">
         <v>102673.53</v>
       </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101019,'Floating','Automobile',24,102673.53);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101019,'Floating','Automobile',24,102673.53,4);</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1006,9 +1072,12 @@
       <c r="G22">
         <v>106168.67</v>
       </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101020,'Floating','Automobile',48,106168.67);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101020,'Floating','Automobile',48,106168.67,4);</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1033,9 +1102,12 @@
       <c r="G23">
         <v>100320.68</v>
       </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101021,'Floating','Automobile',72,100320.68);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101021,'Floating','Automobile',72,100320.68,4);</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1060,9 +1132,12 @@
       <c r="G24">
         <v>107277.97</v>
       </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101022,'Floating','Corporate',36,107277.97);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101022,'Floating','Corporate',36,107277.97,4);</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1087,9 +1162,12 @@
       <c r="G25">
         <v>107509.28</v>
       </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101023,'Fixed','Automobile',120,107509.28);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101023,'Fixed','Automobile',120,107509.28,4);</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1114,9 +1192,12 @@
       <c r="G26">
         <v>104686.2</v>
       </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101024,'Fixed','Housing',24,104686.2);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101024,'Fixed','Housing',24,104686.2,4);</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1141,9 +1222,12 @@
       <c r="G27">
         <v>101053.2</v>
       </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101025,'Fixed','Corporate',96,101053.2);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101025,'Fixed','Corporate',96,101053.2,4);</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1168,9 +1252,12 @@
       <c r="G28">
         <v>100840.78</v>
       </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101026,'Fixed','Corporate',24,100840.78);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101026,'Fixed','Corporate',24,100840.78,4);</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1195,9 +1282,12 @@
       <c r="G29">
         <v>109769.46</v>
       </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101027,'Fixed','Personal',84,109769.46);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101027,'Fixed','Personal',84,109769.46,4);</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -1222,9 +1312,12 @@
       <c r="G30">
         <v>101720.88</v>
       </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101028,'Fixed','Housing',60,101720.88);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101028,'Fixed','Housing',60,101720.88,4);</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -1249,9 +1342,12 @@
       <c r="G31">
         <v>107303.03999999999</v>
       </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101029,'Fixed','Automobile',96,107303.04);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101029,'Fixed','Automobile',96,107303.04,4);</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -1276,9 +1372,12 @@
       <c r="G32">
         <v>103492.6</v>
       </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101030,'Floating','Corporate',72,103492.6);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101030,'Floating','Corporate',72,103492.6,4);</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -1303,9 +1402,12 @@
       <c r="G33">
         <v>105505.91</v>
       </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101031,'Floating','Personal',48,105505.91);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101031,'Floating','Personal',48,105505.91,4);</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -1330,9 +1432,12 @@
       <c r="G34">
         <v>100660.62</v>
       </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101032,'Floating','Corporate',84,100660.62);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101032,'Floating','Corporate',84,100660.62,4);</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -1357,9 +1462,12 @@
       <c r="G35">
         <v>104137.47</v>
       </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101033,'Fixed','Housing',12,104137.47);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101033,'Fixed','Housing',12,104137.47,4);</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -1384,9 +1492,12 @@
       <c r="G36">
         <v>109406.89</v>
       </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101034,'Floating','Automobile',108,109406.89);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101034,'Floating','Automobile',108,109406.89,4);</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -1411,9 +1522,12 @@
       <c r="G37">
         <v>100321.31</v>
       </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101035,'Floating','Personal',24,100321.31);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101035,'Floating','Personal',24,100321.31,4);</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -1438,9 +1552,12 @@
       <c r="G38">
         <v>102803.42</v>
       </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101036,'Fixed','Corporate',108,102803.42);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101036,'Fixed','Corporate',108,102803.42,4);</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -1465,9 +1582,12 @@
       <c r="G39">
         <v>100140.72</v>
       </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101037,'Fixed','Housing',48,100140.72);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101037,'Fixed','Housing',48,100140.72,4);</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -1492,9 +1612,12 @@
       <c r="G40">
         <v>103348.43</v>
       </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101038,'Floating','Personal',96,103348.43);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101038,'Floating','Personal',96,103348.43,4);</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -1519,9 +1642,12 @@
       <c r="G41">
         <v>106750.75</v>
       </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101039,'Fixed','Housing',36,106750.75);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101039,'Fixed','Housing',36,106750.75,4);</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -1546,9 +1672,12 @@
       <c r="G42">
         <v>109316.05</v>
       </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101040,'Fixed','Housing',24,109316.05);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101040,'Fixed','Housing',24,109316.05,4);</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -1573,9 +1702,12 @@
       <c r="G43">
         <v>101799.58</v>
       </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101041,'Fixed','Corporate',72,101799.58);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101041,'Fixed','Corporate',72,101799.58,4);</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -1600,9 +1732,12 @@
       <c r="G44">
         <v>103276.04</v>
       </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101042,'Fixed','Automobile',108,103276.04);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101042,'Fixed','Automobile',108,103276.04,4);</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -1627,9 +1762,12 @@
       <c r="G45">
         <v>101766.24</v>
       </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101043,'Fixed','Housing',36,101766.24);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101043,'Fixed','Housing',36,101766.24,4);</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -1654,9 +1792,12 @@
       <c r="G46">
         <v>109361.77</v>
       </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101044,'Floating','Personal',60,109361.77);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101044,'Floating','Personal',60,109361.77,4);</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -1681,9 +1822,12 @@
       <c r="G47">
         <v>101037.09</v>
       </c>
+      <c r="H47">
+        <v>4</v>
+      </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101045,'Floating','Housing',12,101037.09);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101045,'Floating','Housing',12,101037.09,4);</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -1708,9 +1852,12 @@
       <c r="G48">
         <v>100490.43</v>
       </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101046,'Floating','Corporate',72,100490.43);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101046,'Floating','Corporate',72,100490.43,4);</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
@@ -1735,9 +1882,12 @@
       <c r="G49">
         <v>100409.03</v>
       </c>
+      <c r="H49">
+        <v>4</v>
+      </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101047,'Floating','Automobile',84,100409.03);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101047,'Floating','Automobile',84,100409.03,4);</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -1762,9 +1912,12 @@
       <c r="G50">
         <v>106591.49</v>
       </c>
+      <c r="H50">
+        <v>4</v>
+      </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101048,'Floating','Corporate',72,106591.49);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101048,'Floating','Corporate',72,106591.49,4);</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -1789,9 +1942,12 @@
       <c r="G51">
         <v>108942.56</v>
       </c>
+      <c r="H51">
+        <v>4</v>
+      </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101049,'Fixed','Housing',60,108942.56);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101049,'Fixed','Housing',60,108942.56,4);</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -1816,9 +1972,12 @@
       <c r="G52">
         <v>106577.48</v>
       </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101050,'Floating','Personal',108,106577.48);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101050,'Floating','Personal',108,106577.48,4);</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -1843,9 +2002,12 @@
       <c r="G53">
         <v>104373.35</v>
       </c>
+      <c r="H53">
+        <v>4</v>
+      </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101051,'Floating','Housing',120,104373.35);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101051,'Floating','Housing',120,104373.35,4);</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -1870,9 +2032,12 @@
       <c r="G54">
         <v>104546.7</v>
       </c>
+      <c r="H54">
+        <v>4</v>
+      </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101052,'Fixed','Corporate',84,104546.7);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101052,'Fixed','Corporate',84,104546.7,4);</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -1897,9 +2062,12 @@
       <c r="G55">
         <v>106114.48</v>
       </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101053,'Fixed','Personal',108,106114.48);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101053,'Fixed','Personal',108,106114.48,4);</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -1924,9 +2092,12 @@
       <c r="G56">
         <v>108335.42</v>
       </c>
+      <c r="H56">
+        <v>4</v>
+      </c>
       <c r="J56" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101054,'Fixed','Automobile',72,108335.42);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101054,'Fixed','Automobile',72,108335.42,4);</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -1951,9 +2122,12 @@
       <c r="G57">
         <v>101854.94</v>
       </c>
+      <c r="H57">
+        <v>4</v>
+      </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101055,'Floating','Personal',72,101854.94);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101055,'Floating','Personal',72,101854.94,4);</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -1978,9 +2152,12 @@
       <c r="G58">
         <v>108640.49</v>
       </c>
+      <c r="H58">
+        <v>4</v>
+      </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101056,'Fixed','Personal',120,108640.49);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101056,'Fixed','Personal',120,108640.49,4);</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -2005,9 +2182,12 @@
       <c r="G59">
         <v>101375.16</v>
       </c>
+      <c r="H59">
+        <v>4</v>
+      </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101057,'Fixed','Corporate',72,101375.16);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101057,'Fixed','Corporate',72,101375.16,4);</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -2032,9 +2212,12 @@
       <c r="G60">
         <v>100644.47</v>
       </c>
+      <c r="H60">
+        <v>4</v>
+      </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101058,'Floating','Personal',36,100644.47);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101058,'Floating','Personal',36,100644.47,4);</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -2059,1090 +2242,133 @@
       <c r="G61">
         <v>106058.61</v>
       </c>
+      <c r="H61">
+        <v>4</v>
+      </c>
       <c r="J61" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101059,'Fixed','Personal',84,106058.61);</v>
+        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount], [Lineage Key]) VALUES (101059,'Fixed','Personal',84,106058.61,4);</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>101060</v>
-      </c>
-      <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62">
-        <v>120</v>
-      </c>
-      <c r="F62" s="2">
-        <v>43867</v>
-      </c>
-      <c r="G62">
-        <v>103099.78</v>
-      </c>
-      <c r="J62" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101060,'Floating','Personal',120,103099.78);</v>
-      </c>
+      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>101061</v>
-      </c>
-      <c r="C63" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63">
-        <v>72</v>
-      </c>
-      <c r="F63" s="2">
-        <v>43647</v>
-      </c>
-      <c r="G63">
-        <v>103597.6</v>
-      </c>
-      <c r="J63" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101061,'Fixed','Personal',72,103597.6);</v>
-      </c>
+      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64">
-        <v>101062</v>
-      </c>
-      <c r="C64" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64">
-        <v>24</v>
-      </c>
-      <c r="F64" s="2">
-        <v>43025</v>
-      </c>
-      <c r="G64">
-        <v>106984.42</v>
-      </c>
-      <c r="J64" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101062,'Fixed','Housing',24,106984.42);</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <v>101063</v>
-      </c>
-      <c r="C65" t="s">
-        <v>10</v>
-      </c>
-      <c r="D65" t="s">
-        <v>7</v>
-      </c>
-      <c r="E65">
-        <v>120</v>
-      </c>
-      <c r="F65" s="2">
-        <v>43760</v>
-      </c>
-      <c r="G65">
-        <v>104494.34</v>
-      </c>
-      <c r="J65" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101063,'Floating','Personal',120,104494.34);</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66">
-        <v>101064</v>
-      </c>
-      <c r="C66" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66">
-        <v>84</v>
-      </c>
-      <c r="F66" s="2">
-        <v>43727</v>
-      </c>
-      <c r="G66">
-        <v>109574.39</v>
-      </c>
-      <c r="J66" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101064,'Fixed','Corporate',84,109574.39);</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67">
-        <v>101065</v>
-      </c>
-      <c r="C67" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67">
-        <v>36</v>
-      </c>
-      <c r="F67" s="2">
-        <v>44114</v>
-      </c>
-      <c r="G67">
-        <v>102145.65</v>
-      </c>
-      <c r="J67" t="str">
-        <f t="shared" ref="J67:J101" si="1">"INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES ("&amp;B67&amp;",'"&amp;C67&amp;"','"&amp;D67&amp;"',"&amp;E67&amp;","&amp;G67&amp;");"</f>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101065,'Floating','Corporate',36,102145.65);</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68">
-        <v>101066</v>
-      </c>
-      <c r="C68" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68">
-        <v>72</v>
-      </c>
-      <c r="F68" s="2">
-        <v>43929</v>
-      </c>
-      <c r="G68">
-        <v>100094.01</v>
-      </c>
-      <c r="J68" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101066,'Fixed','Automobile',72,100094.01);</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69">
-        <v>101067</v>
-      </c>
-      <c r="C69" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" t="s">
-        <v>5</v>
-      </c>
-      <c r="E69">
-        <v>120</v>
-      </c>
-      <c r="F69" s="2">
-        <v>43135</v>
-      </c>
-      <c r="G69">
-        <v>101688.94</v>
-      </c>
-      <c r="J69" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101067,'Floating','Housing',120,101688.94);</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70">
-        <v>101068</v>
-      </c>
-      <c r="C70" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" t="s">
-        <v>5</v>
-      </c>
-      <c r="E70">
-        <v>72</v>
-      </c>
-      <c r="F70" s="2">
-        <v>42779</v>
-      </c>
-      <c r="G70">
-        <v>109803.75</v>
-      </c>
-      <c r="J70" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101068,'Floating','Housing',72,109803.75);</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71">
-        <v>101069</v>
-      </c>
-      <c r="C71" t="s">
-        <v>10</v>
-      </c>
-      <c r="D71" t="s">
-        <v>6</v>
-      </c>
-      <c r="E71">
-        <v>96</v>
-      </c>
-      <c r="F71" s="2">
-        <v>43634</v>
-      </c>
-      <c r="G71">
-        <v>106954.79</v>
-      </c>
-      <c r="J71" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101069,'Floating','Automobile',96,106954.79);</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72">
-        <v>101070</v>
-      </c>
-      <c r="C72" t="s">
-        <v>9</v>
-      </c>
-      <c r="D72" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72">
-        <v>60</v>
-      </c>
-      <c r="F72" s="2">
-        <v>43959</v>
-      </c>
-      <c r="G72">
-        <v>109732.55</v>
-      </c>
-      <c r="J72" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101070,'Fixed','Corporate',60,109732.55);</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73">
-        <v>101071</v>
-      </c>
-      <c r="C73" t="s">
-        <v>10</v>
-      </c>
-      <c r="D73" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73">
-        <v>24</v>
-      </c>
-      <c r="F73" s="2">
-        <v>43888</v>
-      </c>
-      <c r="G73">
-        <v>109962.04</v>
-      </c>
-      <c r="J73" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101071,'Floating','Automobile',24,109962.04);</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <v>101072</v>
-      </c>
-      <c r="C74" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74">
-        <v>84</v>
-      </c>
-      <c r="F74" s="2">
-        <v>44066</v>
-      </c>
-      <c r="G74">
-        <v>100801.69</v>
-      </c>
-      <c r="J74" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101072,'Fixed','Automobile',84,100801.69);</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75">
-        <v>101073</v>
-      </c>
-      <c r="C75" t="s">
-        <v>10</v>
-      </c>
-      <c r="D75" t="s">
-        <v>7</v>
-      </c>
-      <c r="E75">
-        <v>108</v>
-      </c>
-      <c r="F75" s="2">
-        <v>43129</v>
-      </c>
-      <c r="G75">
-        <v>106815.22</v>
-      </c>
-      <c r="J75" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101073,'Floating','Personal',108,106815.22);</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76">
-        <v>101074</v>
-      </c>
-      <c r="C76" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76">
-        <v>96</v>
-      </c>
-      <c r="F76" s="2">
-        <v>43608</v>
-      </c>
-      <c r="G76">
-        <v>103272.78</v>
-      </c>
-      <c r="J76" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101074,'Floating','Corporate',96,103272.78);</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77">
-        <v>101075</v>
-      </c>
-      <c r="C77" t="s">
-        <v>9</v>
-      </c>
-      <c r="D77" t="s">
-        <v>6</v>
-      </c>
-      <c r="E77">
-        <v>36</v>
-      </c>
-      <c r="F77" s="2">
-        <v>43442</v>
-      </c>
-      <c r="G77">
-        <v>102302.67</v>
-      </c>
-      <c r="J77" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101075,'Fixed','Automobile',36,102302.67);</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78">
-        <v>101076</v>
-      </c>
-      <c r="C78" t="s">
-        <v>10</v>
-      </c>
-      <c r="D78" t="s">
-        <v>5</v>
-      </c>
-      <c r="E78">
-        <v>60</v>
-      </c>
-      <c r="F78" s="2">
-        <v>43075</v>
-      </c>
-      <c r="G78">
-        <v>108049.06</v>
-      </c>
-      <c r="J78" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101076,'Floating','Housing',60,108049.06);</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79">
-        <v>101077</v>
-      </c>
-      <c r="C79" t="s">
-        <v>9</v>
-      </c>
-      <c r="D79" t="s">
-        <v>7</v>
-      </c>
-      <c r="E79">
-        <v>108</v>
-      </c>
-      <c r="F79" s="2">
-        <v>42604</v>
-      </c>
-      <c r="G79">
-        <v>104264.53</v>
-      </c>
-      <c r="J79" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101077,'Fixed','Personal',108,104264.53);</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80">
-        <v>101078</v>
-      </c>
-      <c r="C80" t="s">
-        <v>10</v>
-      </c>
-      <c r="D80" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80">
-        <v>24</v>
-      </c>
-      <c r="F80" s="2">
-        <v>43474</v>
-      </c>
-      <c r="G80">
-        <v>109014.52</v>
-      </c>
-      <c r="J80" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101078,'Floating','Corporate',24,109014.52);</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="B81">
-        <v>101079</v>
-      </c>
-      <c r="C81" t="s">
-        <v>9</v>
-      </c>
-      <c r="D81" t="s">
-        <v>6</v>
-      </c>
-      <c r="E81">
-        <v>120</v>
-      </c>
-      <c r="F81" s="2">
-        <v>42479</v>
-      </c>
-      <c r="G81">
-        <v>106847.31</v>
-      </c>
-      <c r="J81" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101079,'Fixed','Automobile',120,106847.31);</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="B82">
-        <v>101080</v>
-      </c>
-      <c r="C82" t="s">
-        <v>9</v>
-      </c>
-      <c r="D82" t="s">
-        <v>7</v>
-      </c>
-      <c r="E82">
-        <v>72</v>
-      </c>
-      <c r="F82" s="2">
-        <v>44027</v>
-      </c>
-      <c r="G82">
-        <v>108345.84</v>
-      </c>
-      <c r="J82" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101080,'Fixed','Personal',72,108345.84);</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="B83">
-        <v>101081</v>
-      </c>
-      <c r="C83" t="s">
-        <v>9</v>
-      </c>
-      <c r="D83" t="s">
-        <v>7</v>
-      </c>
-      <c r="E83">
-        <v>96</v>
-      </c>
-      <c r="F83" s="2">
-        <v>43074</v>
-      </c>
-      <c r="G83">
-        <v>103573.7</v>
-      </c>
-      <c r="J83" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101081,'Fixed','Personal',96,103573.7);</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84">
-        <v>83</v>
-      </c>
-      <c r="B84">
-        <v>101082</v>
-      </c>
-      <c r="C84" t="s">
-        <v>10</v>
-      </c>
-      <c r="D84" t="s">
-        <v>7</v>
-      </c>
-      <c r="E84">
-        <v>120</v>
-      </c>
-      <c r="F84" s="2">
-        <v>43903</v>
-      </c>
-      <c r="G84">
-        <v>103728.24</v>
-      </c>
-      <c r="J84" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101082,'Floating','Personal',120,103728.24);</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <v>84</v>
-      </c>
-      <c r="B85">
-        <v>101083</v>
-      </c>
-      <c r="C85" t="s">
-        <v>9</v>
-      </c>
-      <c r="D85" t="s">
-        <v>7</v>
-      </c>
-      <c r="E85">
-        <v>96</v>
-      </c>
-      <c r="F85" s="2">
-        <v>42508</v>
-      </c>
-      <c r="G85">
-        <v>108264.33</v>
-      </c>
-      <c r="J85" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101083,'Fixed','Personal',96,108264.33);</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="B86">
-        <v>101084</v>
-      </c>
-      <c r="C86" t="s">
-        <v>10</v>
-      </c>
-      <c r="D86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86">
-        <v>36</v>
-      </c>
-      <c r="F86" s="2">
-        <v>43578</v>
-      </c>
-      <c r="G86">
-        <v>100255.65</v>
-      </c>
-      <c r="J86" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101084,'Floating','Personal',36,100255.65);</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87">
-        <v>86</v>
-      </c>
-      <c r="B87">
-        <v>101085</v>
-      </c>
-      <c r="C87" t="s">
-        <v>9</v>
-      </c>
-      <c r="D87" t="s">
-        <v>6</v>
-      </c>
-      <c r="E87">
-        <v>12</v>
-      </c>
-      <c r="F87" s="2">
-        <v>44025</v>
-      </c>
-      <c r="G87">
-        <v>105091.82</v>
-      </c>
-      <c r="J87" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101085,'Fixed','Automobile',12,105091.82);</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88">
-        <v>87</v>
-      </c>
-      <c r="B88">
-        <v>101086</v>
-      </c>
-      <c r="C88" t="s">
-        <v>9</v>
-      </c>
-      <c r="D88" t="s">
-        <v>6</v>
-      </c>
-      <c r="E88">
-        <v>12</v>
-      </c>
-      <c r="F88" s="2">
-        <v>43739</v>
-      </c>
-      <c r="G88">
-        <v>105973.29</v>
-      </c>
-      <c r="J88" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101086,'Fixed','Automobile',12,105973.29);</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A89">
-        <v>88</v>
-      </c>
-      <c r="B89">
-        <v>101087</v>
-      </c>
-      <c r="C89" t="s">
-        <v>10</v>
-      </c>
-      <c r="D89" t="s">
-        <v>7</v>
-      </c>
-      <c r="E89">
-        <v>84</v>
-      </c>
-      <c r="F89" s="2">
-        <v>43045</v>
-      </c>
-      <c r="G89">
-        <v>103021.48</v>
-      </c>
-      <c r="J89" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101087,'Floating','Personal',84,103021.48);</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90">
-        <v>89</v>
-      </c>
-      <c r="B90">
-        <v>101088</v>
-      </c>
-      <c r="C90" t="s">
-        <v>9</v>
-      </c>
-      <c r="D90" t="s">
-        <v>7</v>
-      </c>
-      <c r="E90">
-        <v>108</v>
-      </c>
-      <c r="F90" s="2">
-        <v>43056</v>
-      </c>
-      <c r="G90">
-        <v>101881.74</v>
-      </c>
-      <c r="J90" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101088,'Fixed','Personal',108,101881.74);</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A91">
-        <v>90</v>
-      </c>
-      <c r="B91">
-        <v>101089</v>
-      </c>
-      <c r="C91" t="s">
-        <v>9</v>
-      </c>
-      <c r="D91" t="s">
-        <v>5</v>
-      </c>
-      <c r="E91">
-        <v>120</v>
-      </c>
-      <c r="F91" s="2">
-        <v>42421</v>
-      </c>
-      <c r="G91">
-        <v>103090.73</v>
-      </c>
-      <c r="J91" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101089,'Fixed','Housing',120,103090.73);</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92">
-        <v>91</v>
-      </c>
-      <c r="B92">
-        <v>101090</v>
-      </c>
-      <c r="C92" t="s">
-        <v>10</v>
-      </c>
-      <c r="D92" t="s">
-        <v>5</v>
-      </c>
-      <c r="E92">
-        <v>84</v>
-      </c>
-      <c r="F92" s="2">
-        <v>43863</v>
-      </c>
-      <c r="G92">
-        <v>109677.49</v>
-      </c>
-      <c r="J92" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101090,'Floating','Housing',84,109677.49);</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A93">
-        <v>92</v>
-      </c>
-      <c r="B93">
-        <v>101091</v>
-      </c>
-      <c r="C93" t="s">
-        <v>10</v>
-      </c>
-      <c r="D93" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93">
-        <v>12</v>
-      </c>
-      <c r="F93" s="2">
-        <v>42858</v>
-      </c>
-      <c r="G93">
-        <v>109240.26</v>
-      </c>
-      <c r="J93" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101091,'Floating','Automobile',12,109240.26);</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A94">
-        <v>93</v>
-      </c>
-      <c r="B94">
-        <v>101092</v>
-      </c>
-      <c r="C94" t="s">
-        <v>9</v>
-      </c>
-      <c r="D94" t="s">
-        <v>5</v>
-      </c>
-      <c r="E94">
-        <v>24</v>
-      </c>
-      <c r="F94" s="2">
-        <v>44028</v>
-      </c>
-      <c r="G94">
-        <v>100884.75</v>
-      </c>
-      <c r="J94" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101092,'Fixed','Housing',24,100884.75);</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="B95">
-        <v>101093</v>
-      </c>
-      <c r="C95" t="s">
-        <v>9</v>
-      </c>
-      <c r="D95" t="s">
-        <v>6</v>
-      </c>
-      <c r="E95">
-        <v>120</v>
-      </c>
-      <c r="F95" s="2">
-        <v>42911</v>
-      </c>
-      <c r="G95">
-        <v>103963.68</v>
-      </c>
-      <c r="J95" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101093,'Fixed','Automobile',120,103963.68);</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <v>95</v>
-      </c>
-      <c r="B96">
-        <v>101094</v>
-      </c>
-      <c r="C96" t="s">
-        <v>10</v>
-      </c>
-      <c r="D96" t="s">
-        <v>5</v>
-      </c>
-      <c r="E96">
-        <v>60</v>
-      </c>
-      <c r="F96" s="2">
-        <v>43446</v>
-      </c>
-      <c r="G96">
-        <v>108976.46</v>
-      </c>
-      <c r="J96" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101094,'Floating','Housing',60,108976.46);</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <v>96</v>
-      </c>
-      <c r="B97">
-        <v>101095</v>
-      </c>
-      <c r="C97" t="s">
-        <v>9</v>
-      </c>
-      <c r="D97" t="s">
-        <v>5</v>
-      </c>
-      <c r="E97">
-        <v>24</v>
-      </c>
-      <c r="F97" s="2">
-        <v>42884</v>
-      </c>
-      <c r="G97">
-        <v>103617.54</v>
-      </c>
-      <c r="J97" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101095,'Fixed','Housing',24,103617.54);</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <v>97</v>
-      </c>
-      <c r="B98">
-        <v>101096</v>
-      </c>
-      <c r="C98" t="s">
-        <v>9</v>
-      </c>
-      <c r="D98" t="s">
-        <v>7</v>
-      </c>
-      <c r="E98">
-        <v>120</v>
-      </c>
-      <c r="F98" s="2">
-        <v>44011</v>
-      </c>
-      <c r="G98">
-        <v>104275.58</v>
-      </c>
-      <c r="J98" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101096,'Fixed','Personal',120,104275.58);</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <v>98</v>
-      </c>
-      <c r="B99">
-        <v>101097</v>
-      </c>
-      <c r="C99" t="s">
-        <v>9</v>
-      </c>
-      <c r="D99" t="s">
-        <v>8</v>
-      </c>
-      <c r="E99">
-        <v>36</v>
-      </c>
-      <c r="F99" s="2">
-        <v>42539</v>
-      </c>
-      <c r="G99">
-        <v>107392.59</v>
-      </c>
-      <c r="J99" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101097,'Fixed','Corporate',36,107392.59);</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>99</v>
-      </c>
-      <c r="B100">
-        <v>101098</v>
-      </c>
-      <c r="C100" t="s">
-        <v>10</v>
-      </c>
-      <c r="D100" t="s">
-        <v>5</v>
-      </c>
-      <c r="E100">
-        <v>48</v>
-      </c>
-      <c r="F100" s="2">
-        <v>43286</v>
-      </c>
-      <c r="G100">
-        <v>102840.04</v>
-      </c>
-      <c r="J100" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101098,'Floating','Housing',48,102840.04);</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>100</v>
-      </c>
-      <c r="B101">
-        <v>101099</v>
-      </c>
-      <c r="C101" t="s">
-        <v>10</v>
-      </c>
-      <c r="D101" t="s">
-        <v>5</v>
-      </c>
-      <c r="E101">
-        <v>120</v>
-      </c>
-      <c r="F101" s="2">
-        <v>43756</v>
-      </c>
-      <c r="G101">
-        <v>104867.95</v>
-      </c>
-      <c r="J101" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT into [dbo].[Dim_Loans] ([_Source Key], [Interest Rate], [Type of Loan], [Loan Duration], [Loan Principal Amount]) VALUES (101099,'Floating','Housing',120,104867.95);</v>
-      </c>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F101" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>